<commit_message>
Upload timesheet 26/6/18. Also minor deletions in Mers and Gui
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arpit\Desktop\UROP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolaschapman/Documents/UROP/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8F7714-A3A2-4918-BF97-EEEF058B64F4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16245" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -357,16 +356,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -434,7 +433,21 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>43277</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.1875</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.20833333333333334</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>

</xml_diff>

<commit_message>
updated timesheet for monday
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arpit\Desktop\UROP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolaschapman/Documents/UROP/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0134084E-755B-4514-994E-A54F3656C90C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16245" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -357,16 +356,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -502,10 +501,32 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <v>43283</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.20833333333333334</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>43284</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.3923611111111111</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>

</xml_diff>

<commit_message>
timesheet updated for last two days
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -360,7 +360,7 @@
   <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,15 +524,49 @@
       <c r="B11" s="2">
         <v>0.38194444444444442</v>
       </c>
+      <c r="C11" s="2">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="D11" s="2">
         <v>0.3923611111111111</v>
       </c>
+      <c r="E11" s="2">
+        <v>0.23611111111111113</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1">
+        <v>43285</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.20833333333333334</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>43286</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>

</xml_diff>

<commit_message>
Added logging. Focusing now on mgf while cis is put to backburner
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arpit\Desktop\UROP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC94D980-0728-4BBA-AA48-E7E7977ED788}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A21999-AF4D-4BEE-A872-4A5C9290AD2E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16245" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>16/07/2018</t>
   </si>
 </sst>
 </file>
@@ -81,7 +84,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -93,6 +96,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E19"/>
+  <dimension ref="A2:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -665,9 +669,40 @@
       <c r="D18" s="2">
         <v>0.375</v>
       </c>
+      <c r="E18" s="2">
+        <v>0.20833333333333334</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1">
+        <v>43294</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.3125</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Half logic for creating mgf lists. Somehow breaks writing (possibly dangling if?).
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arpit\Desktop\UROP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A21999-AF4D-4BEE-A872-4A5C9290AD2E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA1FCD5-7296-4708-BB34-DFE1F7C4A4CD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16245" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,9 +94,9 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,8 +379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -392,14 +392,14 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -691,7 +691,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -702,6 +702,9 @@
       </c>
       <c r="D20" s="2">
         <v>0.3125</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.14583333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Passed the mgfobj all the way down to the processes
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arpit\Desktop\UROP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5052C0-F53D-4466-9A2D-BB6F44B8ACFF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871ABF1D-11CA-4769-A649-0258D188B64F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16245" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -94,9 +94,11 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E20"/>
+  <dimension ref="A2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -392,14 +394,14 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -691,7 +693,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -705,6 +707,20 @@
       </c>
       <c r="E20" s="2">
         <v>0.17708333333333334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43298</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.3125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated timesheet, stashed experimental changes regarding writer class
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arpit\Desktop\UROP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolaschapman/Documents/UROP/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DF95DC-C310-4EA4-B59D-185BB97E41EF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16245" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -372,16 +371,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -769,6 +768,23 @@
       </c>
       <c r="E24" s="2">
         <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>43308</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.10416666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>